<commit_message>
recreated most of v1.1 on one page
</commit_message>
<xml_diff>
--- a/db/content.xlsx
+++ b/db/content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mk/Documents/GitHub/timeline/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B357148-2DD4-B64D-8386-6F1282D98D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B006A0F7-19C2-A34E-A7A3-D0C40CB11714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14040" yWindow="3200" windowWidth="19560" windowHeight="17800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14040" yWindow="3200" windowWidth="19560" windowHeight="17800" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -410,7 +410,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -452,12 +452,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,7 +741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228A8A84-D9F6-6A4A-9934-A02228219CAA}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -813,7 +812,7 @@
       <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="2">
         <f>INT(LEFT(C2,4))-INT(LEFT(D2,4))</f>
         <v>17</v>
       </c>
@@ -840,7 +839,7 @@
       <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="2">
         <f t="shared" ref="J3:J42" si="0">INT(LEFT(C3,4))-INT(LEFT(D3,4))</f>
         <v>2</v>
       </c>
@@ -865,7 +864,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="4">
+      <c r="J4" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
@@ -890,7 +889,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="4">
+      <c r="J5" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -915,7 +914,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="4">
+      <c r="J6" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -940,7 +939,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="4">
+      <c r="J7" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -967,7 +966,7 @@
       <c r="I8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -992,7 +991,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="4">
+      <c r="J9" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -1017,7 +1016,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="4">
+      <c r="J10" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
@@ -1044,7 +1043,7 @@
       <c r="I11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="2">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
@@ -1069,7 +1068,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="4">
+      <c r="J12" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1094,7 +1093,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="4">
+      <c r="J13" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1119,7 +1118,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="4">
+      <c r="J14" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -1144,7 +1143,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="4">
+      <c r="J15" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
@@ -1169,7 +1168,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="4">
+      <c r="J16" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1194,7 +1193,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="4">
+      <c r="J17" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
@@ -1223,7 +1222,7 @@
       <c r="I18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1248,7 +1247,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="4">
+      <c r="J19" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1279,7 +1278,7 @@
       <c r="I20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1304,7 +1303,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="4">
+      <c r="J21" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1331,7 +1330,7 @@
       <c r="I22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -1358,7 +1357,7 @@
       <c r="I23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1383,7 +1382,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="4">
+      <c r="J24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -1408,7 +1407,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="4">
+      <c r="J25" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1439,7 +1438,7 @@
       <c r="I26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1466,7 +1465,7 @@
       <c r="I27" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1493,7 +1492,7 @@
       <c r="I28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1518,7 +1517,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="4">
+      <c r="J29" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1543,7 +1542,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="4">
+      <c r="J30" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1568,7 +1567,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="4">
+      <c r="J31" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1593,7 +1592,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="4">
+      <c r="J32" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
@@ -1618,7 +1617,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="4">
+      <c r="J33" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1645,7 +1644,7 @@
       <c r="I34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1672,7 +1671,7 @@
       <c r="I35" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1697,7 +1696,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="4">
+      <c r="J36" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
@@ -1726,7 +1725,7 @@
       <c r="I37" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1755,7 +1754,7 @@
       <c r="I38" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1780,7 +1779,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="4">
+      <c r="J39" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -1805,7 +1804,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="4">
+      <c r="J40" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1830,7 +1829,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="4">
+      <c r="J41" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1857,7 +1856,7 @@
       <c r="I42" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1883,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5F732C-24C1-5B48-B08E-FBFAA3C4DF80}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
nine periods updated to float, nicer colors
</commit_message>
<xml_diff>
--- a/db/content.xlsx
+++ b/db/content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mk/Documents/GitHub/timeline/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FF902B-10B6-5C4B-B8DE-B4A56D69B3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1809FB-6A0A-2849-964E-2650969040B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8500" yWindow="1640" windowWidth="25100" windowHeight="19360" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="196">
   <si>
     <t>file</t>
   </si>
@@ -51,9 +51,6 @@
     <t>king</t>
   </si>
   <si>
-    <t>period</t>
-  </si>
-  <si>
     <t>event</t>
   </si>
   <si>
@@ -369,18 +366,9 @@
     <t>note</t>
   </si>
   <si>
-    <t>Wildernis</t>
-  </si>
-  <si>
     <t>Time of the judges</t>
   </si>
   <si>
-    <t>Begin of temple construction 479 years after the exodus</t>
-  </si>
-  <si>
-    <t>1 Kings 6:11</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -535,12 +523,120 @@
   </si>
   <si>
     <t>events</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>text_l</t>
+  </si>
+  <si>
+    <t>text_r</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>1593 to 1473 BCE – 120 years</t>
+  </si>
+  <si>
+    <t>1473-04-01</t>
+  </si>
+  <si>
+    <t>Israel in the wilderness</t>
+  </si>
+  <si>
+    <t>1513 to 1473 BCE – 40 years</t>
+  </si>
+  <si>
+    <t>1473 to 1117 BCE – 356 years</t>
+  </si>
+  <si>
+    <t>1117-04-01</t>
+  </si>
+  <si>
+    <t>479 years to temple construction – 1 Kings 6:1</t>
+  </si>
+  <si>
+    <t>exodus</t>
+  </si>
+  <si>
+    <t>1034-04-01</t>
+  </si>
+  <si>
+    <t>1 Kings 6:1</t>
+  </si>
+  <si>
+    <t>Jesus born 2 BCE</t>
+  </si>
+  <si>
+    <t>Executed Nisan 14th, 33 CE</t>
+  </si>
+  <si>
+    <t>0002-10-01</t>
+  </si>
+  <si>
+    <t>Jesus baptized autumn 29 CE</t>
+  </si>
+  <si>
+    <t>3.5 years of Jesus service</t>
+  </si>
+  <si>
+    <t>69 weeks to the Messiah</t>
+  </si>
+  <si>
+    <t>rebuild Jerusalem 455 BCE</t>
+  </si>
+  <si>
+    <t>Jesus baptized</t>
+  </si>
+  <si>
+    <t>0455-10-01</t>
+  </si>
+  <si>
+    <t>exile</t>
+  </si>
+  <si>
+    <t>Jer. Sieged</t>
+  </si>
+  <si>
+    <t>607 to 537 BCE – 70 years</t>
+  </si>
+  <si>
+    <t>0607-04-01</t>
+  </si>
+  <si>
+    <t>0537-04-01</t>
+  </si>
+  <si>
+    <t>7 times – 2520 years to the Messianic Kingdom 1914 CE</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>0029-10-01</t>
+  </si>
+  <si>
+    <t>0033-04-14</t>
+  </si>
+  <si>
+    <t>1914-10-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="174" formatCode="0.000"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -596,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -608,6 +704,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,21 +919,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>24</v>
@@ -852,7 +950,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -869,7 +967,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -916,18 +1014,18 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B2" s="1">
         <v>-4025.25</v>
@@ -936,12 +1034,12 @@
         <v>-3095.25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B3" s="1">
         <v>-3895.25</v>
@@ -953,7 +1051,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B4" s="1">
         <v>-3790.25</v>
@@ -962,12 +1060,12 @@
         <v>-2885.25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B5" s="1">
         <v>-3700.25</v>
@@ -976,12 +1074,12 @@
         <v>-2790.25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B6" s="1">
         <v>-3630.25</v>
@@ -990,12 +1088,12 @@
         <v>-2735.25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B7" s="1">
         <v>-3565.25</v>
@@ -1007,7 +1105,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B8" s="1">
         <v>-3403.25</v>
@@ -1019,7 +1117,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B9" s="1">
         <v>-3338.25</v>
@@ -1031,7 +1129,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B10" s="1">
         <v>-3151.25</v>
@@ -1043,7 +1141,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B11" s="1">
         <v>-2969.25</v>
@@ -1052,12 +1150,12 @@
         <v>-2019.25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B12" s="1">
         <v>-2467.25</v>
@@ -1066,12 +1164,12 @@
         <v>-1867.25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B13" s="1">
         <v>-2367.25</v>
@@ -1083,7 +1181,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B14" s="1">
         <v>-2332.25</v>
@@ -1095,7 +1193,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B15" s="1">
         <v>-2302.25</v>
@@ -1107,7 +1205,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B16" s="1">
         <v>-2268.25</v>
@@ -1119,7 +1217,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B17" s="1">
         <v>-2238.25</v>
@@ -1131,7 +1229,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B18" s="1">
         <v>-2206.25</v>
@@ -1143,7 +1241,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B19" s="1">
         <v>-2176.25</v>
@@ -1155,7 +1253,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B20" s="1">
         <v>-2147.25</v>
@@ -1167,7 +1265,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B21" s="1">
         <v>-2017.25</v>
@@ -1179,7 +1277,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B22" s="1">
         <v>-1917.25</v>
@@ -1191,7 +1289,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B23" s="1">
         <v>-1857.25</v>
@@ -1203,7 +1301,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B24" s="1">
         <v>-1766.25</v>
@@ -1212,12 +1310,12 @@
         <v>-1656.25</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B25" s="1">
         <v>-1592.25</v>
@@ -1236,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228A8A84-D9F6-6A4A-9934-A02228219CAA}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="125" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O45"/>
+    <sheetView topLeftCell="G1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1258,58 +1356,58 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -1320,14 +1418,14 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1">
         <f>INT(LEFT(C2,4))-INT(LEFT(D2,4))</f>
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2">
         <f>INT(LEFT(K2,4))</f>
@@ -1348,14 +1446,14 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1366,14 +1464,14 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J42" si="0">INT(LEFT(C3,4))-INT(LEFT(D3,4))</f>
         <v>2</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L45" si="1">INT(LEFT(K3,4))</f>
@@ -1394,14 +1492,14 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -1417,7 +1515,7 @@
         <v>41</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
@@ -1438,14 +1536,14 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
@@ -1456,14 +1554,14 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
@@ -1484,14 +1582,14 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
@@ -1507,7 +1605,7 @@
         <v>7</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
@@ -1528,14 +1626,14 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
@@ -1551,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
@@ -1572,14 +1670,14 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1">
         <v>6</v>
@@ -1590,14 +1688,14 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
@@ -1618,14 +1716,14 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1">
         <v>7</v>
@@ -1641,7 +1739,7 @@
         <v>40</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L9">
         <f t="shared" si="1"/>
@@ -1662,14 +1760,14 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1">
         <v>8</v>
@@ -1685,7 +1783,7 @@
         <v>29</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
@@ -1706,14 +1804,14 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="1">
         <v>9</v>
@@ -1724,14 +1822,14 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L11">
         <f t="shared" si="1"/>
@@ -1752,14 +1850,14 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1">
         <v>10</v>
@@ -1775,7 +1873,7 @@
         <v>15</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L12">
         <f t="shared" si="1"/>
@@ -1796,14 +1894,14 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="1">
         <v>11</v>
@@ -1819,7 +1917,7 @@
         <v>16</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L13">
         <f t="shared" si="1"/>
@@ -1840,14 +1938,14 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="1">
         <v>12</v>
@@ -1863,7 +1961,7 @@
         <v>30</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
@@ -1884,14 +1982,14 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="1">
         <v>13</v>
@@ -1907,7 +2005,7 @@
         <v>55</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
@@ -1928,14 +2026,14 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1">
         <v>14</v>
@@ -1951,7 +2049,7 @@
         <v>2</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L16">
         <f t="shared" si="1"/>
@@ -1972,14 +2070,14 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="1">
         <v>15</v>
@@ -1995,7 +2093,7 @@
         <v>31</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
@@ -2016,14 +2114,14 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="1">
         <v>16</v>
@@ -2036,14 +2134,14 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L18">
         <f t="shared" si="1"/>
@@ -2064,14 +2162,14 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="1">
         <v>17</v>
@@ -2087,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
@@ -2108,14 +2206,14 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="1">
         <v>18</v>
@@ -2130,14 +2228,14 @@
         <v>10</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
@@ -2158,14 +2256,14 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="1">
         <v>19</v>
@@ -2181,7 +2279,7 @@
         <v>10</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L21">
         <f t="shared" si="1"/>
@@ -2202,14 +2300,14 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="1">
         <v>17</v>
@@ -2220,14 +2318,14 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L22">
         <f t="shared" si="1"/>
@@ -2248,14 +2346,14 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23" s="1">
         <v>18</v>
@@ -2266,14 +2364,14 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L23">
         <f t="shared" si="1"/>
@@ -2294,14 +2392,14 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="1">
         <v>19</v>
@@ -2317,7 +2415,7 @@
         <v>23</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L24">
         <f t="shared" si="1"/>
@@ -2338,14 +2436,14 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25" s="1">
         <v>20</v>
@@ -2361,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L25">
         <f t="shared" si="1"/>
@@ -2382,14 +2480,14 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26" s="1">
         <v>21</v>
@@ -2404,14 +2502,14 @@
         <v>7</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L26">
         <f t="shared" si="1"/>
@@ -2432,14 +2530,14 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E27" s="1">
         <v>22</v>
@@ -2450,14 +2548,14 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J27" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L27">
         <f t="shared" si="1"/>
@@ -2478,14 +2576,14 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E28" s="1">
         <v>23</v>
@@ -2496,14 +2594,14 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J28" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L28">
         <f t="shared" si="1"/>
@@ -2524,14 +2622,14 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E29" s="1">
         <v>24</v>
@@ -2547,7 +2645,7 @@
         <v>20</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L29">
         <f t="shared" si="1"/>
@@ -2568,14 +2666,14 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="E30" s="1">
         <v>25</v>
@@ -2591,7 +2689,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L30">
         <f t="shared" si="1"/>
@@ -2612,14 +2710,14 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E31" s="1">
         <v>26</v>
@@ -2635,7 +2733,7 @@
         <v>12</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L31">
         <f t="shared" si="1"/>
@@ -2656,14 +2754,14 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E32" s="1">
         <v>27</v>
@@ -2679,7 +2777,7 @@
         <v>29</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L32">
         <f t="shared" si="1"/>
@@ -2700,14 +2798,14 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E33" s="1">
         <v>28</v>
@@ -2723,7 +2821,7 @@
         <v>14</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L33">
         <f t="shared" si="1"/>
@@ -2744,14 +2842,14 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E34" s="1">
         <v>29</v>
@@ -2762,14 +2860,14 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L34">
         <f t="shared" si="1"/>
@@ -2790,14 +2888,14 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E35" s="1">
         <v>30</v>
@@ -2808,14 +2906,14 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J35" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L35">
         <f t="shared" si="1"/>
@@ -2836,14 +2934,14 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E36" s="1">
         <v>31</v>
@@ -2859,7 +2957,7 @@
         <v>41</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L36">
         <f t="shared" si="1"/>
@@ -2880,14 +2978,14 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E37" s="1">
         <v>32</v>
@@ -2900,14 +2998,14 @@
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J37" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L37">
         <f t="shared" si="1"/>
@@ -2928,14 +3026,14 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E38" s="1">
         <v>33</v>
@@ -2948,14 +3046,14 @@
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J38" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L38">
         <f t="shared" si="1"/>
@@ -2976,14 +3074,14 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E39" s="1">
         <v>34</v>
@@ -2999,7 +3097,7 @@
         <v>11</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L39">
         <f t="shared" si="1"/>
@@ -3020,14 +3118,14 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E40" s="1">
         <v>35</v>
@@ -3043,7 +3141,7 @@
         <v>2</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L40">
         <f t="shared" si="1"/>
@@ -3064,14 +3162,14 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E41" s="1">
         <v>36</v>
@@ -3087,7 +3185,7 @@
         <v>20</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L41">
         <f t="shared" si="1"/>
@@ -3108,14 +3206,14 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E42" s="1">
         <v>37</v>
@@ -3126,14 +3224,14 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J42" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L42">
         <f t="shared" si="1"/>
@@ -3154,14 +3252,14 @@
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E43" s="1">
         <v>14</v>
@@ -3173,7 +3271,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="K43" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="L43">
         <f t="shared" si="1"/>
@@ -3194,14 +3292,14 @@
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E44" s="1">
         <v>15</v>
@@ -3213,7 +3311,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="K44" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="L44">
         <f t="shared" si="1"/>
@@ -3234,14 +3332,14 @@
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E45" s="1">
         <v>16</v>
@@ -3253,7 +3351,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="K45" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L45">
         <f t="shared" si="1"/>
@@ -3279,65 +3377,662 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5F732C-24C1-5B48-B08E-FBFAA3C4DF80}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D2" sqref="D2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="5">
+        <v>-1592.75</v>
+      </c>
+      <c r="E2" s="5">
+        <v>-1472.75</v>
+      </c>
+      <c r="F2" s="1">
+        <v>10.9</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="M2">
+        <f>INT(LEFT(L2,4))</f>
+        <v>1473</v>
+      </c>
+      <c r="N2">
+        <f>INT(RIGHT(LEFT(L2,7),2))</f>
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <f>INT(RIGHT(L2,2))</f>
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <f>-M2+1-(12-N2)/12 - (31-O2)/360</f>
+        <v>-1472.75</v>
+      </c>
+      <c r="R2">
+        <v>-1592.75</v>
+      </c>
+      <c r="S2">
+        <v>-1472.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-1512.75</v>
+      </c>
+      <c r="E3" s="5">
+        <v>-1472.75</v>
+      </c>
+      <c r="F3" s="1">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M12" si="0">INT(LEFT(L3,4))</f>
+        <v>1473</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N12" si="1">INT(RIGHT(LEFT(L3,7),2))</f>
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O12" si="2">INT(RIGHT(L3,2))</f>
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P12" si="3">-M3+1-(12-N3)/12 - (31-O3)/360</f>
+        <v>-1472.75</v>
+      </c>
+      <c r="R3">
+        <v>-1512.75</v>
+      </c>
+      <c r="S3">
+        <v>-1472.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1513</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1473</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1473</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="5">
+        <v>-1472.75</v>
+      </c>
+      <c r="E4" s="5">
+        <v>-1116.75</v>
+      </c>
+      <c r="F4" s="1">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
         <v>1117</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1513</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="3"/>
+        <v>-1116.75</v>
+      </c>
+      <c r="R4">
+        <v>-1472.75</v>
+      </c>
+      <c r="S4">
+        <v>-1116.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="5">
+        <v>-1512.75</v>
+      </c>
+      <c r="E5" s="5">
+        <v>-1033.75</v>
+      </c>
+      <c r="F5" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
         <v>1034</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>112</v>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>-1033.75</v>
+      </c>
+      <c r="R5">
+        <v>-1512.75</v>
+      </c>
+      <c r="S5">
+        <v>-1033.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-1.25</v>
+      </c>
+      <c r="E6" s="5">
+        <v>33.800000000000004</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="L6" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>-1.25</v>
+      </c>
+      <c r="R6">
+        <v>-1.25</v>
+      </c>
+      <c r="S6">
+        <v>33.800000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="5">
+        <v>29.866666666666667</v>
+      </c>
+      <c r="E7" s="5">
+        <v>33.800000000000004</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="L7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>905</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="3"/>
+        <v>-904.25</v>
+      </c>
+      <c r="R7" s="5">
+        <v>29.866666666666667</v>
+      </c>
+      <c r="S7">
+        <v>33.800000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="5">
+        <v>-454.25</v>
+      </c>
+      <c r="E8" s="5">
+        <v>29.866666666666667</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>455</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="3"/>
+        <v>-454.25</v>
+      </c>
+      <c r="R8">
+        <v>-454.25</v>
+      </c>
+      <c r="S8" s="5">
+        <v>29.866666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" s="5">
+        <v>-606.75</v>
+      </c>
+      <c r="E9" s="5">
+        <v>-536.75</v>
+      </c>
+      <c r="F9" s="1">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="L9" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>607</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="3"/>
+        <v>-606.75</v>
+      </c>
+      <c r="R9">
+        <v>-606.75</v>
+      </c>
+      <c r="S9">
+        <v>-536.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="5">
+        <v>-606.75</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1914.8666666666666</v>
+      </c>
+      <c r="F10" s="1">
+        <v>21.1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="L10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>829</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="3"/>
+        <v>-828.25</v>
+      </c>
+      <c r="R10">
+        <v>-606.75</v>
+      </c>
+      <c r="S10">
+        <v>1914.8666666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="L11" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>537</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>-536.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="L12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>762</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>-761.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="K14" t="s">
+        <v>192</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14" si="4">INT(LEFT(L14,4))</f>
+        <v>29</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ref="N14" si="5">INT(RIGHT(LEFT(L14,7),2))</f>
+        <v>10</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ref="O14" si="6">INT(RIGHT(L14,2))</f>
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <f>M14+N14/12+O14/30</f>
+        <v>29.866666666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="L15" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ref="M15" si="7">INT(LEFT(L15,4))</f>
+        <v>33</v>
+      </c>
+      <c r="N15">
+        <f t="shared" ref="N15" si="8">INT(RIGHT(LEFT(L15,7),2))</f>
+        <v>4</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ref="O15" si="9">INT(RIGHT(L15,2))</f>
+        <v>14</v>
+      </c>
+      <c r="P15">
+        <f>M15+N15/12+O15/30</f>
+        <v>33.800000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="L16" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ref="M16" si="10">INT(LEFT(L16,4))</f>
+        <v>1914</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ref="N16" si="11">INT(RIGHT(LEFT(L16,7),2))</f>
+        <v>10</v>
+      </c>
+      <c r="O16">
+        <f t="shared" ref="O16" si="12">INT(RIGHT(L16,2))</f>
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <f>M16+N16/12+O16/30</f>
+        <v>1914.8666666666666</v>
       </c>
     </row>
   </sheetData>
@@ -3357,13 +4052,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3383,24 +4078,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B2">
         <v>2370</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>